<commit_message>
Debugging ingest for chapter 2 and fixing other issues with logging and CLI
</commit_message>
<xml_diff>
--- a/data/templates/dukes_ch_2.xlsx
+++ b/data/templates/dukes_ch_2.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\PycharmProjects\uk_energy_data_api\data\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291B852C-E989-4DD1-B0B1-FDB1DBF87F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD4624D-CF2C-4DDF-862F-58EFB52813B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2.1" sheetId="1" r:id="rId1"/>
     <sheet name="2.2" sheetId="2" r:id="rId2"/>
     <sheet name="2.3" sheetId="3" r:id="rId3"/>
     <sheet name="2.4" sheetId="4" r:id="rId4"/>
+    <sheet name="2.1.1" sheetId="5" r:id="rId5"/>
+    <sheet name="2.1.2" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="123">
   <si>
     <t>Production</t>
   </si>
@@ -267,9 +269,6 @@
     <t>Total stocks at end of year [note 6]</t>
   </si>
   <si>
-    <t>lable</t>
-  </si>
-  <si>
     <t>Surface mining</t>
   </si>
   <si>
@@ -328,6 +327,79 @@
   </si>
   <si>
     <t>GWh</t>
+  </si>
+  <si>
+    <t>Total production</t>
+  </si>
+  <si>
+    <t>Surface mining [note 2][note 3]</t>
+  </si>
+  <si>
+    <t>Imports [note 4]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exports </t>
+  </si>
+  <si>
+    <t>Distributed</t>
+  </si>
+  <si>
+    <t>Undistributed</t>
+  </si>
+  <si>
+    <t>Trade</t>
+  </si>
+  <si>
+    <t>Total inland consumption of coal</t>
+  </si>
+  <si>
+    <t>Collieries</t>
+  </si>
+  <si>
+    <t>Power stations [note 1]</t>
+  </si>
+  <si>
+    <t>Coke ovens and blast furnaces</t>
+  </si>
+  <si>
+    <t>Other solid fuel plants [note 3]</t>
+  </si>
+  <si>
+    <t>Gas works</t>
+  </si>
+  <si>
+    <t>Total consumption by fuel producers 
+[note 1]</t>
+  </si>
+  <si>
+    <t>Total sector consumption</t>
+  </si>
+  <si>
+    <t>Fuel producers</t>
+  </si>
+  <si>
+    <t>Final users</t>
+  </si>
+  <si>
+    <t>Other solid fuels</t>
+  </si>
+  <si>
+    <t>Coke and breeze</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Cokes and breeze</t>
+  </si>
+  <si>
+    <t>Total inland consumption</t>
+  </si>
+  <si>
+    <t>Power stations</t>
+  </si>
+  <si>
+    <t>Other solid fuel plants</t>
   </si>
 </sst>
 </file>
@@ -335,7 +407,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="31" x14ac:knownFonts="1">
     <font>
@@ -886,7 +958,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -896,11 +968,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="62">
     <cellStyle name="20% - Colore 1 2" xfId="19" xr:uid="{AB28A018-B116-4807-AD53-D336FCC42037}"/>
@@ -1342,7 +1417,7 @@
         <v>57</v>
       </c>
       <c r="F1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G1" t="s">
         <v>58</v>
@@ -2691,8 +2766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B64E19E-3D03-4D18-A8D3-625E632D0784}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2707,7 +2782,7 @@
         <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
         <v>55</v>
@@ -2719,7 +2794,7 @@
         <v>57</v>
       </c>
       <c r="F1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G1" t="s">
         <v>58</v>
@@ -2782,13 +2857,13 @@
         <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s">
         <v>64</v>
@@ -2805,13 +2880,13 @@
         <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G5" t="s">
         <v>64</v>
@@ -3041,7 +3116,7 @@
         <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G15" t="s">
         <v>64</v>
@@ -3722,16 +3797,16 @@
         <v>75</v>
       </c>
       <c r="C45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G45" t="s">
         <v>64</v>
@@ -3745,13 +3820,13 @@
         <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F46" t="s">
         <v>12</v>
@@ -3768,13 +3843,13 @@
         <v>76</v>
       </c>
       <c r="C47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F47" t="s">
         <v>76</v>
@@ -3791,10 +3866,10 @@
         <v>77</v>
       </c>
       <c r="C48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E48" t="s">
         <v>77</v>
@@ -3814,16 +3889,16 @@
         <v>78</v>
       </c>
       <c r="C49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E49" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F49" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G49" t="s">
         <v>64</v>
@@ -3864,10 +3939,10 @@
         <v>57</v>
       </c>
       <c r="F1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -3890,7 +3965,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -3913,7 +3988,7 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -3936,7 +4011,7 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -3959,7 +4034,7 @@
         <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -3982,7 +4057,7 @@
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -4005,7 +4080,7 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -4028,7 +4103,7 @@
         <v>60</v>
       </c>
       <c r="G8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -4051,7 +4126,7 @@
         <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -4074,7 +4149,7 @@
         <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -4097,7 +4172,7 @@
         <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -4120,7 +4195,7 @@
         <v>19</v>
       </c>
       <c r="G12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -4143,7 +4218,7 @@
         <v>26</v>
       </c>
       <c r="G13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -4166,7 +4241,7 @@
         <v>27</v>
       </c>
       <c r="G14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -4189,7 +4264,7 @@
         <v>28</v>
       </c>
       <c r="G15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -4212,7 +4287,7 @@
         <v>29</v>
       </c>
       <c r="G16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -4235,7 +4310,7 @@
         <v>30</v>
       </c>
       <c r="G17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -4258,7 +4333,7 @@
         <v>63</v>
       </c>
       <c r="G18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -4281,7 +4356,7 @@
         <v>47</v>
       </c>
       <c r="G19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -4289,19 +4364,19 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4309,7 +4384,7 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
         <v>59</v>
@@ -4324,7 +4399,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -4347,7 +4422,7 @@
         <v>2</v>
       </c>
       <c r="G22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -4370,7 +4445,7 @@
         <v>3</v>
       </c>
       <c r="G23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -4393,7 +4468,7 @@
         <v>62</v>
       </c>
       <c r="G24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -4416,7 +4491,7 @@
         <v>6</v>
       </c>
       <c r="G25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -4439,7 +4514,7 @@
         <v>7</v>
       </c>
       <c r="G26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -4462,7 +4537,7 @@
         <v>60</v>
       </c>
       <c r="G27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -4485,7 +4560,7 @@
         <v>9</v>
       </c>
       <c r="G28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -4508,7 +4583,7 @@
         <v>10</v>
       </c>
       <c r="G29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -4531,7 +4606,7 @@
         <v>16</v>
       </c>
       <c r="G30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -4554,7 +4629,7 @@
         <v>17</v>
       </c>
       <c r="G31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -4577,7 +4652,7 @@
         <v>19</v>
       </c>
       <c r="G32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -4600,7 +4675,7 @@
         <v>26</v>
       </c>
       <c r="G33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -4623,7 +4698,7 @@
         <v>27</v>
       </c>
       <c r="G34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -4646,7 +4721,7 @@
         <v>28</v>
       </c>
       <c r="G35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -4669,7 +4744,7 @@
         <v>29</v>
       </c>
       <c r="G36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -4677,19 +4752,19 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D37" t="s">
+        <v>90</v>
+      </c>
+      <c r="E37" t="s">
+        <v>90</v>
+      </c>
+      <c r="G37" t="s">
         <v>91</v>
-      </c>
-      <c r="E37" t="s">
-        <v>91</v>
-      </c>
-      <c r="G37" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -4712,7 +4787,7 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -4735,7 +4810,7 @@
         <v>2</v>
       </c>
       <c r="G39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -4758,7 +4833,7 @@
         <v>3</v>
       </c>
       <c r="G40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -4781,7 +4856,7 @@
         <v>62</v>
       </c>
       <c r="G41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -4804,7 +4879,7 @@
         <v>7</v>
       </c>
       <c r="G42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -4827,7 +4902,7 @@
         <v>60</v>
       </c>
       <c r="G43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -4850,7 +4925,7 @@
         <v>9</v>
       </c>
       <c r="G44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -4873,7 +4948,7 @@
         <v>10</v>
       </c>
       <c r="G45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -4896,7 +4971,7 @@
         <v>19</v>
       </c>
       <c r="G46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -4919,7 +4994,7 @@
         <v>22</v>
       </c>
       <c r="G47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -4942,7 +5017,7 @@
         <v>26</v>
       </c>
       <c r="G48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -4965,7 +5040,7 @@
         <v>27</v>
       </c>
       <c r="G49" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -4988,7 +5063,7 @@
         <v>28</v>
       </c>
       <c r="G50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -5011,7 +5086,7 @@
         <v>63</v>
       </c>
       <c r="G51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -5034,7 +5109,7 @@
         <v>47</v>
       </c>
       <c r="G52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -5042,19 +5117,19 @@
         <v>58</v>
       </c>
       <c r="B53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C53" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -5066,7 +5141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FB2FF3-339D-4212-9F35-64EC4D87C409}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A38" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
@@ -5092,10 +5167,10 @@
         <v>57</v>
       </c>
       <c r="F1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H1" t="s">
         <v>58</v>
@@ -5121,10 +5196,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -5147,10 +5222,10 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -5173,10 +5248,10 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -5184,7 +5259,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
         <v>59</v>
@@ -5199,10 +5274,10 @@
         <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -5225,10 +5300,10 @@
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -5251,10 +5326,10 @@
         <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -5277,10 +5352,10 @@
         <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -5303,10 +5378,10 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -5329,10 +5404,10 @@
         <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -5355,10 +5430,10 @@
         <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -5381,10 +5456,10 @@
         <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -5407,10 +5482,10 @@
         <v>19</v>
       </c>
       <c r="G13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -5433,10 +5508,10 @@
         <v>16</v>
       </c>
       <c r="G14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -5459,10 +5534,10 @@
         <v>17</v>
       </c>
       <c r="G15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -5485,10 +5560,10 @@
         <v>24</v>
       </c>
       <c r="G16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -5511,10 +5586,10 @@
         <v>25</v>
       </c>
       <c r="G17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -5537,10 +5612,10 @@
         <v>26</v>
       </c>
       <c r="G18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -5563,10 +5638,10 @@
         <v>27</v>
       </c>
       <c r="G19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -5589,10 +5664,10 @@
         <v>28</v>
       </c>
       <c r="G20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -5615,10 +5690,10 @@
         <v>29</v>
       </c>
       <c r="G21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -5641,10 +5716,10 @@
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -5667,10 +5742,10 @@
         <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -5693,10 +5768,10 @@
         <v>3</v>
       </c>
       <c r="G24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -5704,7 +5779,7 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
         <v>59</v>
@@ -5719,10 +5794,10 @@
         <v>6</v>
       </c>
       <c r="G25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -5745,10 +5820,10 @@
         <v>7</v>
       </c>
       <c r="G26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -5771,10 +5846,10 @@
         <v>60</v>
       </c>
       <c r="G27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -5797,10 +5872,10 @@
         <v>9</v>
       </c>
       <c r="G28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -5823,10 +5898,10 @@
         <v>10</v>
       </c>
       <c r="G29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -5849,10 +5924,10 @@
         <v>11</v>
       </c>
       <c r="G30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -5875,10 +5950,10 @@
         <v>14</v>
       </c>
       <c r="G31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -5901,10 +5976,10 @@
         <v>24</v>
       </c>
       <c r="G32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -5927,10 +6002,10 @@
         <v>19</v>
       </c>
       <c r="G33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -5953,10 +6028,10 @@
         <v>16</v>
       </c>
       <c r="G34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -5979,10 +6054,10 @@
         <v>17</v>
       </c>
       <c r="G35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -6005,10 +6080,10 @@
         <v>24</v>
       </c>
       <c r="G36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -6031,10 +6106,10 @@
         <v>25</v>
       </c>
       <c r="G37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -6057,10 +6132,10 @@
         <v>26</v>
       </c>
       <c r="G38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -6083,10 +6158,10 @@
         <v>27</v>
       </c>
       <c r="G39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -6109,10 +6184,10 @@
         <v>28</v>
       </c>
       <c r="G40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -6135,10 +6210,10 @@
         <v>29</v>
       </c>
       <c r="G41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -6161,10 +6236,10 @@
         <v>0</v>
       </c>
       <c r="G42" t="s">
+        <v>97</v>
+      </c>
+      <c r="H42" t="s">
         <v>98</v>
-      </c>
-      <c r="H42" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -6172,7 +6247,7 @@
         <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C43" t="s">
         <v>61</v>
@@ -6187,10 +6262,10 @@
         <v>26</v>
       </c>
       <c r="G43" t="s">
+        <v>97</v>
+      </c>
+      <c r="H43" t="s">
         <v>98</v>
-      </c>
-      <c r="H43" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -6213,10 +6288,10 @@
         <v>28</v>
       </c>
       <c r="G44" t="s">
+        <v>97</v>
+      </c>
+      <c r="H44" t="s">
         <v>98</v>
-      </c>
-      <c r="H44" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -6239,10 +6314,10 @@
         <v>29</v>
       </c>
       <c r="G45" t="s">
+        <v>97</v>
+      </c>
+      <c r="H45" t="s">
         <v>98</v>
-      </c>
-      <c r="H45" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -6265,10 +6340,480 @@
         <v>52</v>
       </c>
       <c r="G46" t="s">
+        <v>97</v>
+      </c>
+      <c r="H46" t="s">
         <v>98</v>
       </c>
-      <c r="H46" t="s">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7C0385-B298-465E-BE89-9B3F85EFE2C7}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>99</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32669E1E-5E72-47A9-A395-802B05B6BA7C}">
+  <dimension ref="A1:P14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="24.44140625" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" t="s">
+        <v>120</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" t="s">
+        <v>120</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F14" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>